<commit_message>
Release v0.1.0-beta: Fix validation errors and update canonical URL
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-onc-problem-type.xlsx
+++ b/docs/CodeSystem-onc-problem-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>0.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -48,16 +48,19 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-28T01:24:36+00:00</t>
+    <t>2025-12-26T14:13:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,6 +75,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Code system for categorizing types of nursing problems</t>
+  </si>
+  <si>
     <t>Purpose</t>
   </si>
   <si>
@@ -81,6 +87,9 @@
     <t>Case Sensitive</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Value Set (all codes)</t>
   </si>
   <si>
@@ -105,25 +114,49 @@
     <t>Count</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
     <t>nursing-diagnosis</t>
   </si>
   <si>
     <t>Nursing Diagnosis</t>
+  </si>
+  <si>
+    <t>A clinical judgment about individual, family, or community responses to actual or potential health problems</t>
+  </si>
+  <si>
+    <t>risk-diagnosis</t>
+  </si>
+  <si>
+    <t>Risk Diagnosis</t>
+  </si>
+  <si>
+    <t>A clinical judgment about an individual's vulnerability to developing an undesirable health condition</t>
+  </si>
+  <si>
+    <t>health-promotion</t>
+  </si>
+  <si>
+    <t>Health Promotion Diagnosis</t>
+  </si>
+  <si>
+    <t>A clinical judgment about motivation to increase wellbeing</t>
   </si>
 </sst>
 </file>
@@ -319,98 +352,104 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -420,7 +459,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,29 +467,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>